<commit_message>
added validation of JSON response for POST
</commit_message>
<xml_diff>
--- a/target/classes/com/qa/testdata/FreeCrmTestData.xlsx
+++ b/target/classes/com/qa/testdata/FreeCrmTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>TestCaseno</t>
   </si>
@@ -30,34 +30,7 @@
     <t>yes</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>kerala</t>
-  </si>
-  <si>
     <t>Text</t>
-  </si>
-  <si>
-    <t>data one</t>
-  </si>
-  <si>
-    <t>data two</t>
-  </si>
-  <si>
-    <t>vellamunda</t>
-  </si>
-  <si>
-    <t>wayanad</t>
-  </si>
-  <si>
-    <t>malabar</t>
-  </si>
-  <si>
-    <t>how are you doing?</t>
-  </si>
-  <si>
-    <t>which is this place</t>
   </si>
   <si>
     <t>message</t>
@@ -382,10 +355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A3" sqref="A3:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -402,7 +375,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -413,95 +386,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
         <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>